<commit_message>
loader success popup added
</commit_message>
<xml_diff>
--- a/DMS/ImportItemAssignedToLocation.xlsx
+++ b/DMS/ImportItemAssignedToLocation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>PartnerCode</t>
   </si>
@@ -28,9 +28,6 @@
     <t>I000037</t>
   </si>
   <si>
-    <t>I000042</t>
-  </si>
-  <si>
     <t>I000055</t>
   </si>
   <si>
@@ -50,6 +47,78 @@
   </si>
   <si>
     <t>MaximumQty</t>
+  </si>
+  <si>
+    <t>PCode2</t>
+  </si>
+  <si>
+    <t>I000056</t>
+  </si>
+  <si>
+    <t>PCode3</t>
+  </si>
+  <si>
+    <t>I000057</t>
+  </si>
+  <si>
+    <t>PCode4</t>
+  </si>
+  <si>
+    <t>I000058</t>
+  </si>
+  <si>
+    <t>PCode5</t>
+  </si>
+  <si>
+    <t>I000059</t>
+  </si>
+  <si>
+    <t>PCode6</t>
+  </si>
+  <si>
+    <t>I000060</t>
+  </si>
+  <si>
+    <t>PCode7</t>
+  </si>
+  <si>
+    <t>I000061</t>
+  </si>
+  <si>
+    <t>PCode8</t>
+  </si>
+  <si>
+    <t>I000062</t>
+  </si>
+  <si>
+    <t>PCode9</t>
+  </si>
+  <si>
+    <t>I000063</t>
+  </si>
+  <si>
+    <t>PCode10</t>
+  </si>
+  <si>
+    <t>I000064</t>
+  </si>
+  <si>
+    <t>DRGP-0000002</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>I000038</t>
+  </si>
+  <si>
+    <t>DRGP-0000003</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>I000039</t>
   </si>
 </sst>
 </file>
@@ -391,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,18 +484,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -440,13 +509,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -457,18 +526,239 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>0</v>
       </c>
     </row>

</xml_diff>